<commit_message>
Fixed graph, added overall conclusions and added code/data
</commit_message>
<xml_diff>
--- a/data/TOTAL - Goodstransport_mld_ton.xlsx
+++ b/data/TOTAL - Goodstransport_mld_ton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelme\TIL6022\Pythongroup8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991CAF0A-8797-4720-973F-8F0D941E38FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB43126B-0980-4904-B2FA-92B66C926F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederenvervoer_mld_ton_eigen" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Trend</t>
-  </si>
-  <si>
     <t>Inland Waterways</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -896,33 +896,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added data and V2 File
</commit_message>
<xml_diff>
--- a/data/TOTAL - Goodstransport_mld_ton.xlsx
+++ b/data/TOTAL - Goodstransport_mld_ton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelme\TIL6022\Pythongroup8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991CAF0A-8797-4720-973F-8F0D941E38FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869EC64-C3CF-45D0-8E78-9B432464FA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederenvervoer_mld_ton_eigen" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Trend</t>
-  </si>
-  <si>
     <t>Inland Waterways</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -897,32 +897,32 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>